<commit_message>
4 Tables with Data  in Excel Added
</commit_message>
<xml_diff>
--- a/eskaysoft.gst.data.xlsx
+++ b/eskaysoft.gst.data.xlsx
@@ -4,30 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="19815" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="360" windowWidth="19815" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="STATEMST" sheetId="1" r:id="rId1"/>
-    <sheet name="District" sheetId="2" r:id="rId2"/>
+    <sheet name="Schmast" sheetId="3" r:id="rId1"/>
+    <sheet name="SubSchmast" sheetId="4" r:id="rId2"/>
+    <sheet name="Statemast" sheetId="1" r:id="rId3"/>
+    <sheet name="Distmast" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Database">STATEMST!$A$1:$C$37</definedName>
+    <definedName name="_xlnm.Database">Statemast!$B$1:$D$37</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>ZONE</t>
-  </si>
-  <si>
-    <t>CODE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="127">
   <si>
     <t>ANDHRA PRADESH</t>
   </si>
@@ -152,10 +145,262 @@
     <t>MIZORAM</t>
   </si>
   <si>
-    <t>District name</t>
-  </si>
-  <si>
-    <t>District code</t>
+    <t>stateid</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>statename</t>
+  </si>
+  <si>
+    <t>statecode</t>
+  </si>
+  <si>
+    <t>KAMAREDDY</t>
+  </si>
+  <si>
+    <t>GUNTUR</t>
+  </si>
+  <si>
+    <t>KRISHNA</t>
+  </si>
+  <si>
+    <t>PRAKASAM</t>
+  </si>
+  <si>
+    <t>NELLORE</t>
+  </si>
+  <si>
+    <t>CHITTOR</t>
+  </si>
+  <si>
+    <t>CUDDAPAH</t>
+  </si>
+  <si>
+    <t>KURNOOL</t>
+  </si>
+  <si>
+    <t>MAHABOOBNAGAR</t>
+  </si>
+  <si>
+    <t>NALGONDA</t>
+  </si>
+  <si>
+    <t>HYDERABAD</t>
+  </si>
+  <si>
+    <t>ADILABAD</t>
+  </si>
+  <si>
+    <t>NIZAMABAD</t>
+  </si>
+  <si>
+    <t>MEDAK</t>
+  </si>
+  <si>
+    <t>WARANGAL</t>
+  </si>
+  <si>
+    <t>KHAMMAM</t>
+  </si>
+  <si>
+    <t>EAST GODAVARI</t>
+  </si>
+  <si>
+    <t>WEST GODAVARI</t>
+  </si>
+  <si>
+    <t>VIJAYANAGARAM</t>
+  </si>
+  <si>
+    <t>SRIKAKULAM</t>
+  </si>
+  <si>
+    <t>VISAKAPATNAM</t>
+  </si>
+  <si>
+    <t>RANGAREDDY</t>
+  </si>
+  <si>
+    <t>ANANTAPUR</t>
+  </si>
+  <si>
+    <t>KAREEMNAGAR</t>
+  </si>
+  <si>
+    <t>JAGTIAL</t>
+  </si>
+  <si>
+    <t>distid</t>
+  </si>
+  <si>
+    <t>distname</t>
+  </si>
+  <si>
+    <t>CAPITAL ACCOUNTS</t>
+  </si>
+  <si>
+    <t>UNSECURED LOANS</t>
+  </si>
+  <si>
+    <t>FIXED ASSETS</t>
+  </si>
+  <si>
+    <t>BANKS</t>
+  </si>
+  <si>
+    <t>CASH BALANCES</t>
+  </si>
+  <si>
+    <t>EXPENSES</t>
+  </si>
+  <si>
+    <t>DEPOSITES,BANK LOANS &amp; CHITS</t>
+  </si>
+  <si>
+    <t>SUNDRY DEBTORS</t>
+  </si>
+  <si>
+    <t>SUNDRY CREDITORS</t>
+  </si>
+  <si>
+    <t>OTHER THAN TRADE DEBTORS</t>
+  </si>
+  <si>
+    <t>VAT PAYABLE</t>
+  </si>
+  <si>
+    <t>OTHER THAN TRADE CREDITORS</t>
+  </si>
+  <si>
+    <t>PUR &amp; SALES</t>
+  </si>
+  <si>
+    <t>SGST TAX</t>
+  </si>
+  <si>
+    <t>CGST TAX</t>
+  </si>
+  <si>
+    <t>IGST TAX</t>
+  </si>
+  <si>
+    <t>CST PAYABLE</t>
+  </si>
+  <si>
+    <t>GST PAYABLE/RECEIVABLE</t>
+  </si>
+  <si>
+    <t>CURRENT LIABILITES</t>
+  </si>
+  <si>
+    <t>CURRENT ASSETS</t>
+  </si>
+  <si>
+    <t>GST PAID ON RCM</t>
+  </si>
+  <si>
+    <t>IGST PAID ON RCM</t>
+  </si>
+  <si>
+    <t>CGST PAID ON RCM</t>
+  </si>
+  <si>
+    <t>SGST PAID ON RCM</t>
+  </si>
+  <si>
+    <t>Liabilites</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Profit and Loss</t>
+  </si>
+  <si>
+    <t>Trading</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>schid</t>
+  </si>
+  <si>
+    <t>schname</t>
+  </si>
+  <si>
+    <t>schindex</t>
+  </si>
+  <si>
+    <t>schtype</t>
+  </si>
+  <si>
+    <t>VAT PUR &amp; SALES</t>
+  </si>
+  <si>
+    <t>GST PUR &amp; SALES</t>
+  </si>
+  <si>
+    <t>EXPENSES OTHER THAN GST</t>
+  </si>
+  <si>
+    <t>EXPENSES (GST)</t>
+  </si>
+  <si>
+    <t>EXPENSES (RCM)</t>
+  </si>
+  <si>
+    <t>IGST ON TRADING</t>
+  </si>
+  <si>
+    <t>IGST ON EXPENSES</t>
+  </si>
+  <si>
+    <t>IGST ON RCM</t>
+  </si>
+  <si>
+    <t>CGST ON TRADING</t>
+  </si>
+  <si>
+    <t>CGST ON EXPENSES</t>
+  </si>
+  <si>
+    <t>CGST ON RCM</t>
+  </si>
+  <si>
+    <t>SGST ON TRADING</t>
+  </si>
+  <si>
+    <t>SGST ON EXPENSES</t>
+  </si>
+  <si>
+    <t>SGST ON RCM</t>
+  </si>
+  <si>
+    <t>GST PAYABLE/RECEIVABLE(TRADING)</t>
+  </si>
+  <si>
+    <t>GST PAYABLE/RECEIVABLE(RCM)</t>
+  </si>
+  <si>
+    <t>GST LATE FEE INPUT(ADVANCE PAID)</t>
+  </si>
+  <si>
+    <t>subschid</t>
+  </si>
+  <si>
+    <t>subschname</t>
+  </si>
+  <si>
+    <t>subschindex</t>
+  </si>
+  <si>
+    <t>credit</t>
+  </si>
+  <si>
+    <t>debit</t>
   </si>
 </sst>
 </file>
@@ -640,9 +885,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -978,452 +1224,1908 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
+      <c r="B8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="1">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="1">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="1">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="1">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="1">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="1">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="1">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
+      <c r="B25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="1">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="1">
-        <v>15</v>
+      <c r="D25" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="B2:E25">
+    <sortCondition ref="E1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="1">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="1">
+        <v>13</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="1">
+        <v>14</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="1">
+        <v>14</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="1">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="1">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="1">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="1">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="1">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="1">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="1">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="1">
+        <v>18</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="1">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="1">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="1">
+        <v>19</v>
+      </c>
+      <c r="D28" s="1">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="1">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="1">
+        <v>21</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="1">
+        <v>22</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="1">
+        <v>23</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="1">
+        <v>24</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F33">
+    <sortCondition ref="C1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="1">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="1">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="1">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="1">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>29</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="1">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="1">
+        <v>31</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="1">
+        <v>32</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
+        <v>33</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1">
+        <v>34</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="1">
+        <v>35</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1">
+        <v>36</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>37</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:E37">
+    <sortCondition ref="E1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:C1048576">
+    <sortCondition ref="B7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>